<commit_message>
Need to come back to z score and central limit theorem
</commit_message>
<xml_diff>
--- a/Homework/JulyCentralLimitHW.xlsx
+++ b/Homework/JulyCentralLimitHW.xlsx
@@ -1,30 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\edxtake2module1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anguyen\Documents\GitHub\stats-edx\Homework\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3691E75-B53C-4BBD-9B6F-76153C2AF213}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8310"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Homework 3_7</t>
   </si>
@@ -39,16 +46,77 @@
   </si>
   <si>
     <t>3.        I have 500 potential customers who come to my candy store each day. Seventy percent of the customers buy no pieces of candy, 15 percent buy one piece, 10 percent buy two pieces, and 5 percent buy three pieces. What is the chance that I sell at least 280 pieces of candy in a day?</t>
+  </si>
+  <si>
+    <t>n=500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mean </t>
+  </si>
+  <si>
+    <t>variance</t>
+  </si>
+  <si>
+    <t>mean on each die</t>
+  </si>
+  <si>
+    <t>var</t>
+  </si>
+  <si>
+    <t>stdev</t>
+  </si>
+  <si>
+    <t>mean for 400</t>
+  </si>
+  <si>
+    <t>&gt;1450</t>
+  </si>
+  <si>
+    <t>z = (x - mean)/std</t>
+  </si>
+  <si>
+    <t>z = -0.5</t>
+  </si>
+  <si>
+    <t>mean = 70</t>
+  </si>
+  <si>
+    <t>std = 10</t>
+  </si>
+  <si>
+    <t>c1</t>
+  </si>
+  <si>
+    <t>c2</t>
+  </si>
+  <si>
+    <t>mean = 75</t>
+  </si>
+  <si>
+    <t>std = 8</t>
+  </si>
+  <si>
+    <t>z = 1.5</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>std</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="169" formatCode="0.0000000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,6 +149,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -105,10 +180,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="7"/>
@@ -119,9 +195,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -398,51 +477,59 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:E19"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="61.26953125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="13.26953125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.1796875" style="3"/>
+    <col min="1" max="1" width="61.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:7" ht="94.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="111" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="129.5" x14ac:dyDescent="0.35">
+      <c r="C4" s="8">
+        <f>1-_xlfn.NORM.DIST(20,0,(252*(1.5^2))^(1/2),TRUE)</f>
+        <v>0.20047632682095895</v>
+      </c>
+      <c r="D4" s="3">
+        <f>(252*(1.5^2))^(1/2)</f>
+        <v>23.811761799581316</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="131.25" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -451,7 +538,7 @@
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -460,8 +547,10 @@
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A8" s="4"/>
+    <row r="8" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -469,17 +558,24 @@
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
+    <row r="9" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4">
+        <f>(0.7*0+0.15*1+0.1*2+0.05*3)*500</f>
+        <v>250</v>
+      </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A10" s="4"/>
+    <row r="10" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -487,7 +583,7 @@
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -496,8 +592,11 @@
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A12" s="4"/>
+    <row r="12" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
+        <f>1-_xlfn.NORM.DIST(10,8.22,1.1,TRUE)</f>
+        <v>5.2811710001670509E-2</v>
+      </c>
       <c r="B12" s="4"/>
       <c r="C12" s="6"/>
       <c r="D12" s="4"/>
@@ -505,7 +604,7 @@
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="6"/>
@@ -514,60 +613,693 @@
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
+    <row r="14" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="4">
+        <v>3.5</v>
+      </c>
       <c r="C14" s="6"/>
       <c r="D14" s="4"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
+    <row r="15" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="4">
+        <v>2.9166669999999999</v>
+      </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
     </row>
-    <row r="16" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
+    <row r="16" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="4">
+        <f>SQRT(B15)</f>
+        <v>1.7078252252499375</v>
+      </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
-      <c r="E17" s="5"/>
+      <c r="E17" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
     </row>
-    <row r="18" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
+    <row r="18" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="4">
+        <f>B14*400</f>
+        <v>1400</v>
+      </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="7">
+        <f>B15*400</f>
+        <v>1166.6668</v>
+      </c>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
     </row>
+    <row r="20" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="3">
+        <f>B19^(1/2)</f>
+        <v>34.15650450499875</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <f>1-_xlfn.NORM.DIST(1450,B18,B20,TRUE)</f>
+        <v>7.1617465192515661E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <f>STANDARDIZE(95,70,10)</f>
+        <v>2.5</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D25" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="9">
+        <f>_xlfn.NORM.DIST(390*25,400*25,(400*25)^(1/2),TRUE)</f>
+        <v>6.2096653257761331E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C27" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D28" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C29" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D30" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D31" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C32" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" s="3">
+        <f>1.5*8 +75</f>
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{147A73F4-8B62-415B-930C-4E76A9407979}">
+  <dimension ref="A1:E100"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2">
+        <f>AVERAGE(A1:A100)</f>
+        <v>50.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3">
+        <f>_xlfn.STDEV.S(A1:A100)</f>
+        <v>29.011491975882016</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="E5">
+        <f>-0.5*E3 + E2</f>
+        <v>35.994254012058988</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>